<commit_message>
revisiting visual protein, correcting pathways
</commit_message>
<xml_diff>
--- a/data_picrust/output_base/bacteria_classification.xlsx
+++ b/data_picrust/output_base/bacteria_classification.xlsx
@@ -15,6 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="checked_usual" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="core_usual" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="all_three" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="components" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,100 +447,68 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Clostridium</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>214</v>
+          <t>Acetobacterium</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Corynebacterium</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>229</v>
+          <t>Bacillus</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Novosphingobium</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>491</v>
+          <t>Clostridium</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Streptococcus</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>687</v>
+          <t>Corynebacterium</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Thiobacillus</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>727</v>
+          <t>Desulfobacterium</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Acetobacterium</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
+          <t>Desulfobulbus</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bacillus</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>113</v>
+          <t>Desulfotomaculum</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Desulfotomaculum</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>270</v>
+          <t>Desulfovibrio</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Desulfovibrio</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>271</v>
+          <t>Gallionella</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -548,78 +517,54 @@
           <t>Micrococcus</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>462</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Propionibacterium</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>572</v>
+          <t>Novosphingobium</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Pseudomonas</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>587</v>
+          <t>Propionibacterium</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Staphylococcus</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>683</v>
+          <t>Pseudomonas</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Desulfobacterium</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>264</v>
+          <t>Shewanella</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Desulfobulbus</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>265</v>
+          <t>Staphylococcus</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Gallionella</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>332</v>
+          <t>Streptococcus</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Shewanella</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>656</v>
+          <t>Thiobacillus</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -633,7 +578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -647,11 +592,6 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -659,9 +599,6 @@
           <t>Brachybacterium</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>140</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -669,9 +606,6 @@
           <t>Brevibacterium</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>145</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -679,9 +613,6 @@
           <t>Bulleidia</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>154</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -689,9 +620,6 @@
           <t>Enterococcus</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>300</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -699,9 +627,6 @@
           <t>Gelria</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>334</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -709,9 +634,6 @@
           <t>Legionella</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>408</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -719,9 +641,6 @@
           <t>Mycobacterium</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>470</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -729,9 +648,6 @@
           <t>Mycoplana</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>471</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -739,9 +655,6 @@
           <t>Neisseria</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>474</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -749,9 +662,6 @@
           <t>Oerskovia</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>497</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -759,9 +669,6 @@
           <t>Opitutus</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>503</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -769,9 +676,6 @@
           <t>Oxobacter</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>512</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -779,9 +683,6 @@
           <t>Paracoccus</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>526</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -789,9 +690,6 @@
           <t>Phenylobacterium</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>549</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -799,9 +697,6 @@
           <t>Porphyrobacter</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>564</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -809,9 +704,6 @@
           <t>Prevotella</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>566</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -819,9 +711,6 @@
           <t>Pseudarthrobacter</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>583</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -829,18 +718,12 @@
           <t>Pseudoalteromonas</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>584</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
           <t>Tepidimonas</t>
         </is>
-      </c>
-      <c r="B20" t="n">
-        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:A47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,11 +751,6 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -880,9 +758,6 @@
           <t>Achromobacter</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -890,9 +765,6 @@
           <t>Acidisoma</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -900,9 +772,6 @@
           <t>Acidovorax</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -910,9 +779,6 @@
           <t>Aestuariimicrobium</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -920,9 +786,6 @@
           <t>Afipia</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -930,9 +793,6 @@
           <t>Anoxybacillus</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>89</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -940,9 +800,6 @@
           <t>Beta_proteobacterium</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>130</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -950,9 +807,6 @@
           <t>Blastomonas</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>136</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -960,9 +814,6 @@
           <t>Bradyrhizobium</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>143</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -970,9 +821,6 @@
           <t>Brevundimonas</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>146</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -980,9 +828,6 @@
           <t>Candidatus_desulforudis</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>177</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -990,9 +835,6 @@
           <t>Caulobacter</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>198</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1000,9 +842,6 @@
           <t>Chryseobacterium</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>206</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1010,9 +849,6 @@
           <t>Clostridium_sensu_stricto_12</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>217</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1020,9 +856,6 @@
           <t>Cutibacterium</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>238</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1030,9 +863,6 @@
           <t>Dechloromonas</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>245</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1040,9 +870,6 @@
           <t>Desulfomicrobium</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>267</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1050,9 +877,6 @@
           <t>Desulfosporosinus</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>269</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1060,9 +884,6 @@
           <t>Enhydrobacter</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>296</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1070,9 +891,6 @@
           <t>Erysipelothrix</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>304</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1080,9 +898,6 @@
           <t>Flavisolibacter</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>322</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1090,9 +905,6 @@
           <t>Geothrix</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>344</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1100,9 +912,6 @@
           <t>Herbaspirillum</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>360</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1110,9 +919,6 @@
           <t>Hydrogenophaga</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>371</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1120,9 +926,6 @@
           <t>Methylocystis</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>449</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1130,188 +933,131 @@
           <t>Nitrospira</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>484</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Phreatobacter</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>550</v>
+          <t>Oxalobacteraceae_unclassified</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Propionivibrio</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>575</v>
+          <t>Phreatobacter</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Pseudorhodoferax</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>589</v>
+          <t>Propionivibrio</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Pseudoxanthomonas</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>591</v>
+          <t>Pseudorhodoferax</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ralstonia</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>596</v>
+          <t>Pseudoxanthomonas</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ruminiclostridium_1</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>634</v>
+          <t>Ralstonia</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Sediminibacterium</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>647</v>
+          <t>Ruminiclostridium_1</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Silanimonas</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>659</v>
+          <t>Sediminibacterium</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Simplicispira</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>660</v>
+          <t>Silanimonas</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Smithella</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>664</v>
+          <t>Simplicispira</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sphingobium</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>671</v>
+          <t>Smithella</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sphingomonas</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>674</v>
+          <t>Sphingobium</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sphingopyxis</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>676</v>
+          <t>Sphingomonas</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Syntrophus</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>705</v>
+          <t>Sphingopyxis</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Tessaracoccus</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>715</v>
+          <t>Syntrophus</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Thermincola</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>719</v>
+          <t>Tessaracoccus</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Treponema</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>731</v>
+          <t>Thermincola</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Oxalobacteraceae_unclassified</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>853</v>
+          <t>Treponema</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1320,18 +1066,12 @@
           <t>Variovorax</t>
         </is>
       </c>
-      <c r="B46" t="n">
-        <v>863</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
           <t>Wchb1-05</t>
         </is>
-      </c>
-      <c r="B47" t="n">
-        <v>867</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1085,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1359,11 +1099,6 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1371,9 +1106,6 @@
           <t>Desulfobacterium</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>264</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1381,9 +1113,6 @@
           <t>Desulfobulbus</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>265</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1391,18 +1120,12 @@
           <t>Gallionella</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>332</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>Shewanella</t>
         </is>
-      </c>
-      <c r="B5" t="n">
-        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -1416,7 +1139,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1430,11 +1153,6 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1442,9 +1160,6 @@
           <t>Azospira</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>110</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1452,9 +1167,6 @@
           <t>Clostridium</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>214</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1462,9 +1174,6 @@
           <t>Corynebacterium</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>229</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1472,9 +1181,6 @@
           <t>Halomonas</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>354</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1482,9 +1188,6 @@
           <t>Novosphingobium</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>491</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1492,18 +1195,12 @@
           <t>Psb-m-3</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>581</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>Streptococcus</t>
         </is>
-      </c>
-      <c r="B8" t="n">
-        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -1517,7 +1214,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1531,11 +1228,6 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1543,9 +1235,6 @@
           <t>Clostridium</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>214</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1553,9 +1242,6 @@
           <t>Corynebacterium</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>229</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1563,9 +1249,6 @@
           <t>Novosphingobium</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>491</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1573,18 +1256,12 @@
           <t>Streptococcus</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>687</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
           <t>Thiobacillus</t>
         </is>
-      </c>
-      <c r="B6" t="n">
-        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -1598,7 +1275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1612,130 +1289,89 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Clostridium</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>214</v>
+          <t>Acetobacterium</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Corynebacterium</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>229</v>
+          <t>Bacillus</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Novosphingobium</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>491</v>
+          <t>Clostridium</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Streptococcus</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>687</v>
+          <t>Corynebacterium</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Acetobacterium</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>6</v>
+          <t>Desulfotomaculum</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bacillus</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>113</v>
+          <t>Desulfovibrio</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Desulfotomaculum</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>270</v>
+          <t>Micrococcus</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Desulfovibrio</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>271</v>
+          <t>Novosphingobium</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Micrococcus</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>462</v>
+          <t>Propionibacterium</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Propionibacterium</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>572</v>
+          <t>Pseudomonas</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Pseudomonas</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>587</v>
+          <t>Staphylococcus</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Staphylococcus</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>683</v>
+          <t>Streptococcus</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1749,7 +1385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1763,11 +1399,6 @@
           <t>Genus</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1775,9 +1406,6 @@
           <t>Clostridium</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>214</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1785,9 +1413,6 @@
           <t>Corynebacterium</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>229</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1795,9 +1420,6 @@
           <t>Novosphingobium</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>491</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1805,8 +1427,276 @@
           <t>Streptococcus</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>687</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Genus</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Acetobacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Azospira</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bacillus</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Brachybacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brevibacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bulleidia</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Corynebacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Desulfotomaculum</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Desulfovibrio</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Enterococcus</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Gelria</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Halomonas</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Legionella</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Micrococcus</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mycobacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Mycoplana</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Neisseria</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Novosphingobium</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Oerskovia</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Opitutus</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Oxobacter</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Paracoccus</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Phenylobacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Porphyrobacter</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Prevotella</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Propionibacterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Psb-m-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Pseudarthrobacter</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Pseudoalteromonas</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Pseudomonas</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Staphylococcus</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Streptococcus</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Tepidimonas</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Thiobacillus</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>